<commit_message>
minor fixes in the test case
</commit_message>
<xml_diff>
--- a/test/preprocessing/Inventory_of_tags.xlsx
+++ b/test/preprocessing/Inventory_of_tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/hmm_smast/test/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734790F4-7058-904F-99BF-AA52278858A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498A4451-4C6D-2A4C-A611-77900B7A3B5B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="18060" windowWidth="27640" windowHeight="16940" xr2:uid="{368BD445-8588-FF47-BFEA-5BC7CD5831B9}"/>
+    <workbookView xWindow="2060" yWindow="4100" windowWidth="27640" windowHeight="16940" xr2:uid="{368BD445-8588-FF47-BFEA-5BC7CD5831B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,12 +42,6 @@
     <t>VEMCO</t>
   </si>
   <si>
-    <t>VEMCO SERIAL</t>
-  </si>
-  <si>
-    <t>VEMCO ID</t>
-  </si>
-  <si>
     <t>DATE TAGGED</t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>FISH WAS RELEASED DEAD, STILL HAS ACOUSTIC TAG IN IT. FISHERMAN WAS SURE IT WAS DEAD.</t>
+  </si>
+  <si>
+    <t>RELEASE_LAT</t>
+  </si>
+  <si>
+    <t>RELEASE_LONG</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,7 @@
   <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +673,7 @@
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -713,70 +713,70 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -814,22 +814,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="4">
-        <v>1075012</v>
+        <v>42.524745000000003</v>
       </c>
       <c r="G8" s="4">
-        <v>59666</v>
+        <v>-70.695231000000007</v>
       </c>
       <c r="H8" s="5">
         <v>40305</v>
@@ -841,14 +841,14 @@
         <v>73</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L8" s="4">
         <v>4</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O8" s="5">
         <v>40324</v>
@@ -857,7 +857,7 @@
         <v>19</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R8" s="8">
         <v>42.401111111111113</v>
@@ -866,7 +866,7 @@
         <v>-70.37166666666667</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U8" s="9">
         <v>15</v>
@@ -875,10 +875,10 @@
         <v>29.28</v>
       </c>
       <c r="W8" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y8" s="4">
         <v>73</v>
@@ -887,7 +887,7 @@
         <v>19</v>
       </c>
       <c r="AA8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:27" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -895,22 +895,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" s="4">
-        <v>1075013</v>
+        <v>42.524745000000003</v>
       </c>
       <c r="G9" s="4">
-        <v>59667</v>
+        <v>-70.695231000000007</v>
       </c>
       <c r="H9" s="5">
         <v>40305</v>
@@ -922,14 +922,14 @@
         <v>81</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L9" s="4">
         <v>4</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O9" s="5">
         <v>40333</v>
@@ -938,7 +938,7 @@
         <v>28</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R9" s="8">
         <v>42.41</v>
@@ -947,7 +947,7 @@
         <v>-70.368333333333339</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U9" s="9">
         <v>15</v>
@@ -956,10 +956,10 @@
         <v>29.09</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y9" s="11">
         <v>72.39</v>
@@ -968,7 +968,7 @@
         <v>23</v>
       </c>
       <c r="AA9" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -986,22 +986,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F12" s="4">
-        <v>1088948</v>
+        <v>42.524745000000003</v>
       </c>
       <c r="G12" s="4">
-        <v>2220</v>
+        <v>-70.695231000000007</v>
       </c>
       <c r="H12" s="5">
         <v>40309</v>
@@ -1013,14 +1013,14 @@
         <v>87</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L12" s="4">
         <v>4</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O12" s="5">
         <v>40337</v>
@@ -1029,7 +1029,7 @@
         <v>28</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R12" s="8">
         <v>42.397222222222226</v>
@@ -1038,7 +1038,7 @@
         <v>-70.375</v>
       </c>
       <c r="T12" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U12" s="9">
         <v>15</v>
@@ -1047,10 +1047,10 @@
         <v>29.07</v>
       </c>
       <c r="W12" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y12" s="4">
         <v>-999</v>
@@ -1059,7 +1059,7 @@
         <v>18</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:27" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1067,22 +1067,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F13" s="4">
-        <v>1088945</v>
+        <v>42.524745000000003</v>
       </c>
       <c r="G13" s="4">
-        <v>2217</v>
+        <v>-70.695231000000007</v>
       </c>
       <c r="H13" s="5">
         <v>40309</v>
@@ -1094,14 +1094,14 @@
         <v>85</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L13" s="4">
         <v>5</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O13" s="5">
         <v>40365</v>
@@ -1110,7 +1110,7 @@
         <v>56</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R13" s="8">
         <v>42.261876111111114</v>
@@ -1119,7 +1119,7 @@
         <v>-70.547353888888892</v>
       </c>
       <c r="T13" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U13" s="9">
         <v>30</v>
@@ -1128,10 +1128,10 @@
         <v>30.97</v>
       </c>
       <c r="W13" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Y13" s="4">
         <v>86</v>
@@ -1140,7 +1140,7 @@
         <v>17</v>
       </c>
       <c r="AA13" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>